<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2024-11-16.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2024-11-16.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2024-11-16.xlsx
@@ -520,6 +520,9 @@
       <c r="C11" t="str">
         <v>268_猩红泡泡_spray red_Rosa rugosa Thunb._10stems</v>
       </c>
+      <c r="F11" t="str">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -581,7 +584,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>020203510101010100</v>
+        <v>0202035101010101010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>